<commit_message>
Examen Final 2 - 11 de diciembre de 2022 - Lap HP
Se elabora el examen final segunda vuelta para el curso de Física Computacional.
</commit_message>
<xml_diff>
--- a/Combinacion/Grupo_2023_1.xlsx
+++ b/Combinacion/Grupo_2023_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gusto\OneDrive\Documentos\FComputacional\Combinacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{104595E4-64BC-4DB6-9A26-8C0FC3E6C5F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430659BD-FE06-481E-A863-C6B9BF46D59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="108">
   <si>
     <t>Facultad de Ciencias</t>
   </si>
@@ -1002,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="N15" sqref="N15"/>
+    <sheetView tabSelected="1" topLeftCell="D6" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1434,8 +1434,8 @@
         <f t="shared" si="3"/>
         <v>6.7183011363636362</v>
       </c>
-      <c r="N13" s="19" t="s">
-        <v>104</v>
+      <c r="N13" s="19">
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.2">
@@ -1653,29 +1653,29 @@
         <v>6.42</v>
       </c>
       <c r="H18" s="18">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I18" s="20">
         <f t="shared" si="2"/>
-        <v>7.218</v>
+        <v>8.468</v>
       </c>
       <c r="J18" s="32">
         <f t="shared" si="4"/>
-        <v>0.46916999999999998</v>
+        <v>0.55042000000000002</v>
       </c>
       <c r="K18" s="32">
         <v>0.30068181818181816</v>
       </c>
       <c r="L18" s="20">
         <f t="shared" si="5"/>
-        <v>7.6985181818181818</v>
+        <v>8.5110181818181818</v>
       </c>
       <c r="M18" s="20">
         <f t="shared" si="3"/>
-        <v>8.3812227272727267</v>
+        <v>9.1937227272727267</v>
       </c>
       <c r="N18" s="19">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.2">

</xml_diff>